<commit_message>
xls file change of import sample file
</commit_message>
<xml_diff>
--- a/src/assets/sample-files/trial-balance-sample.xlsx
+++ b/src/assets/sample-files/trial-balance-sample.xlsx
@@ -11,11 +11,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Account Name</t>
   </si>
   <si>
+    <t>Group Name/Group Unique Name</t>
+  </si>
+  <si>
     <t>Credit</t>
   </si>
   <si>
@@ -25,18 +28,30 @@
     <t>Mihir Sharma</t>
   </si>
   <si>
+    <t>sundrydebtors</t>
+  </si>
+  <si>
     <t>Suhan Khan</t>
   </si>
   <si>
+    <t>sundrycreditors</t>
+  </si>
+  <si>
     <t>Mahaveer Jain</t>
   </si>
   <si>
     <t>wages</t>
   </si>
   <si>
+    <t>Operating cost</t>
+  </si>
+  <si>
     <t>Rent</t>
   </si>
   <si>
+    <t>Other Income</t>
+  </si>
+  <si>
     <t>Comission</t>
   </si>
   <si>
@@ -46,7 +61,13 @@
     <t>Cash</t>
   </si>
   <si>
+    <t>current asset</t>
+  </si>
+  <si>
     <t>HDFC Loan</t>
+  </si>
+  <si>
+    <t>Current liabilities</t>
   </si>
   <si>
     <t>Taxes</t>
@@ -67,11 +88,9 @@
       <sz val="11.0"/>
       <name val="Arial"/>
     </font>
+    <font/>
     <font>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -89,7 +108,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border/>
     <border>
       <left style="thin">
@@ -105,36 +124,6 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
@@ -144,19 +133,19 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -179,107 +168,166 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="18.57"/>
+    <col customWidth="1" min="2" max="2" width="24.43"/>
+    <col customWidth="1" min="3" max="3" width="21.43"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="45.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="5">
         <v>500.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="5">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="5">
         <v>100.0</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="5">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="3">
         <v>10325.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5">
+        <v>9</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="3">
         <v>9000.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="5">
+        <v>11</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3">
         <v>5000.0</v>
       </c>
-      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="5">
+        <v>13</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="3">
         <v>90000.0</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="5">
+        <v>14</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="3">
         <v>5000.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="5">
+        <v>15</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="3">
         <v>9635.0</v>
       </c>
-      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="5">
+        <v>17</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="3">
         <v>900000.0</v>
       </c>
-      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="5">
+        <v>19</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="3">
         <v>500.0</v>
       </c>
-      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>